<commit_message>
bugs detected and eliminated
</commit_message>
<xml_diff>
--- a/months/jan23/jan23.xlsx
+++ b/months/jan23/jan23.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="184">
   <si>
     <t xml:space="preserve">DATE</t>
   </si>
@@ -339,148 +339,341 @@
     <t xml:space="preserve">30*</t>
   </si>
   <si>
-    <t xml:space="preserve">{&lt;.22: 3*, &lt;.23: 2*, &gt;.23: 0}</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="utkal"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">&lt;.22": "3*", "&lt;.23": "2*", "&gt;.23": 0}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="utkal"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">1": 50, "2": 0}</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">50*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">40*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"+": {"CDIF": 50, "P": 25}, "-": {"CDIF": 0, "P": -25}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"&lt;.23": "1*", "&gt;.23": 0}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"&lt;.23": "3*", "&gt;.23": 0}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dutyFalse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">True</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"&lt;.22": "2*", "&lt;.23": "1*", "&gt;.23": 0}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"1": 50, "2": 0}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"+": {"CDIF": 100, "P": 50}, "-": {"CDIFP": 0}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"&lt;.23": "1*", "&gt;.23": 0, "&gt;.0": "-1*"}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">False</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="utkal"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="utkal"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">: 1, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="utkal"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="utkal"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">: 1.25, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="utkal"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="utkal"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">: 1.5}</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">duty_8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WEAK1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WEAK2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KGD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Egr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EGR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LERA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">long_box100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">long_box50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">enc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fine50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fine100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">250</t>
+  </si>
+  <si>
+    <t xml:space="preserve">200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">450</t>
+  </si>
+  <si>
+    <t xml:space="preserve">150</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ПЕРЕДЕЛАЙ ЧЕРЕЗ ДРУГОЙ ЕХСЕЛ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">350</t>
+  </si>
+  <si>
+    <t xml:space="preserve">300</t>
+  </si>
+  <si>
+    <t xml:space="preserve">400</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-300</t>
+  </si>
+  <si>
+    <t xml:space="preserve">итог</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-150</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{&lt;22: 3*, &lt;23: 2*, &gt;23: 0}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{&lt;22: 2*, &lt;23: 1*, &gt;23: 0*}</t>
   </si>
   <si>
     <t xml:space="preserve">{1: 50, 2: 0}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">40*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"+": {"CDIF": 50, "P": 25}, "-": {"CDIF": 0, "P": -25}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{&lt;.23: 1*, &gt;.23: 0}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{&lt;.23: 3*, &gt;.23: 0}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dutyFalse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">True</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{&lt;.22: 2*, &lt;2.3: 1*, &gt;2.3: 0*}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"+": {"CDIF": 100, "P": 50}, "-": {"CDIFP": 0}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{&lt;.23: 1*, &gt;.23: 0, &gt;.0: -1*}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">False</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{1: 1, 2: 1.25, 3: 1.5}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">duty_8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WEAK1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WEAK2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KGD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#</t>
-  </si>
-  <si>
-    <t xml:space="preserve">!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">price</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Egr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lera</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EGR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LERA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">long_box100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">long_box50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">enc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fine50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fine100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">250</t>
-  </si>
-  <si>
-    <t xml:space="preserve">200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">450</t>
-  </si>
-  <si>
-    <t xml:space="preserve">150</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ПЕРЕДЕЛАЙ ЧЕРЕЗ ДРУГОЙ ЕХСЕЛ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">350</t>
-  </si>
-  <si>
-    <t xml:space="preserve">300</t>
-  </si>
-  <si>
-    <t xml:space="preserve">400</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-300</t>
-  </si>
-  <si>
-    <t xml:space="preserve">итог</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-150</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{&lt;22: 3*, &lt;23: 2*, &gt;23: 0}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{&lt;22: 2*, &lt;23: 1*, &gt;23: 0*}</t>
   </si>
   <si>
     <t xml:space="preserve">{&gt;22: 3*, 22-23: 2*, &gt;23: 0}</t>
@@ -587,7 +780,7 @@
     <numFmt numFmtId="167" formatCode="0.00"/>
     <numFmt numFmtId="168" formatCode="h:mm"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -609,6 +802,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="utkal"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -766,7 +966,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -790,7 +990,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -798,7 +998,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -914,11 +1114,11 @@
   </sheetPr>
   <dimension ref="A1:AD33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S17" activeCellId="0" sqref="S17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I5" activeCellId="0" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="4.43"/>
@@ -946,7 +1146,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="7.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="2" width="7.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="7.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="5.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="5.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="7.43"/>
   </cols>
   <sheetData>
@@ -3089,24 +3289,25 @@
   </sheetPr>
   <dimension ref="A1:X13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S13" activeCellId="0" sqref="S13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="S1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="U16" activeCellId="0" sqref="U16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="27.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="34.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="34.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="0" width="18.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="49.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="20.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="17" style="0" width="20.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="0" width="24.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="24.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="33.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="17" style="0" width="24.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="47.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="33.77"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3183,7 +3384,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
         <v>101</v>
       </c>
@@ -3342,7 +3543,7 @@
         <v>114</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>105</v>
@@ -3372,13 +3573,13 @@
         <v>50</v>
       </c>
       <c r="N4" s="9" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="O4" s="7" t="n">
         <v>50</v>
       </c>
       <c r="P4" s="7" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="Q4" s="7" t="n">
         <v>0</v>
@@ -3387,13 +3588,13 @@
         <v>111</v>
       </c>
       <c r="S4" s="9" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="T4" s="9" t="n">
         <v>0</v>
       </c>
       <c r="U4" s="7" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="V4" s="7" t="s">
         <v>109</v>
@@ -3407,7 +3608,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="11" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B5" s="7" t="n">
         <v>0</v>
@@ -3479,7 +3680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="21.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="12" t="s">
         <v>5</v>
       </c>
@@ -3514,25 +3715,25 @@
         <v>1</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="N6" s="7" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="O6" s="7" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="P6" s="7" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="Q6" s="7" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="R6" s="7" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="S6" s="7" t="n">
         <v>1</v>
@@ -3555,7 +3756,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="12" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B7" s="7" t="n">
         <v>0.75</v>
@@ -3629,7 +3830,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="13" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B8" s="7" t="n">
         <v>1.25</v>
@@ -3703,7 +3904,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="13" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B9" s="7" t="n">
         <v>1.5</v>
@@ -3851,7 +4052,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="14" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B11" s="7" t="n">
         <v>0.75</v>
@@ -3999,12 +4200,12 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
       <c r="D13" s="9" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E13" s="9"/>
       <c r="F13" s="9"/>
@@ -4012,32 +4213,32 @@
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
       <c r="J13" s="9" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="K13" s="9"/>
       <c r="L13" s="9" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="M13" s="9" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="N13" s="9" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="O13" s="9" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="P13" s="9" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="Q13" s="9" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="R13" s="9" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="S13" s="9" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="T13" s="9"/>
       <c r="U13" s="9"/>
@@ -4067,7 +4268,7 @@
       <selection pane="topLeft" activeCell="I29" activeCellId="0" sqref="I29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="12.14"/>
@@ -4077,19 +4278,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C1" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="G1" s="16" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4098,7 +4299,7 @@
         <v>#REF!</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F2" s="2" t="n">
         <f aca="false">D2*C2</f>
@@ -4109,7 +4310,7 @@
         <v>0</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="O2" s="0" t="n">
         <v>100</v>
@@ -4121,7 +4322,7 @@
         <v>#REF!</v>
       </c>
       <c r="N3" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="O3" s="0" t="n">
         <v>50</v>
@@ -4133,7 +4334,7 @@
         <v>#REF!</v>
       </c>
       <c r="N4" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="O4" s="0" t="n">
         <v>50</v>
@@ -4145,13 +4346,13 @@
         <v>#REF!</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="N5" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="O5" s="0" t="n">
         <v>-50</v>
@@ -4163,10 +4364,10 @@
         <v>#REF!</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="N6" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="O6" s="0" t="n">
         <v>-100</v>
@@ -4178,7 +4379,7 @@
         <v>#REF!</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4187,7 +4388,7 @@
         <v>#REF!</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4196,10 +4397,10 @@
         <v>#REF!</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4220,10 +4421,10 @@
         <v>#REF!</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4244,10 +4445,10 @@
         <v>#REF!</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4274,10 +4475,10 @@
         <v>#REF!</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4292,10 +4493,10 @@
         <v>#REF!</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4304,7 +4505,7 @@
         <v>#REF!</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4313,10 +4514,10 @@
         <v>#REF!</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4331,7 +4532,7 @@
         <v>#REF!</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4346,30 +4547,30 @@
         <v>#REF!</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E28" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E30" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="16" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B31" s="18"/>
       <c r="C31" s="16"/>
       <c r="D31" s="18" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E31" s="18" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -4402,7 +4603,7 @@
       <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.15"/>
@@ -4410,7 +4611,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="9" width="7.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="9" width="7.7"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4427,31 +4628,31 @@
         <v>113</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F1" s="12" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="I1" s="13" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="J1" s="14" t="s">
         <v>76</v>
       </c>
       <c r="K1" s="14" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="L1" s="15" t="s">
         <v>64</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4497,13 +4698,13 @@
         <v>7</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>-50</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>-50</v>
@@ -4535,13 +4736,13 @@
         <v>8</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>104</v>
+        <v>152</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>0</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>104</v>
+        <v>152</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>0</v>
@@ -4611,13 +4812,13 @@
         <v>10</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>-50</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>-50</v>
@@ -4796,7 +4997,7 @@
         <v>1</v>
       </c>
       <c r="M10" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4837,7 +5038,7 @@
         <v>1</v>
       </c>
       <c r="N11" s="0" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4857,7 +5058,7 @@
         <v>-50</v>
       </c>
       <c r="F12" s="20" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="G12" s="20" t="n">
         <v>1.5</v>
@@ -4878,7 +5079,7 @@
         <v>1</v>
       </c>
       <c r="M12" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4898,7 +5099,7 @@
         <v>-50</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="G13" s="7" t="n">
         <v>1.5</v>
@@ -4919,7 +5120,7 @@
         <v>1</v>
       </c>
       <c r="M13" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4927,19 +5128,19 @@
         <v>18</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C14" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="F14" s="7" t="s">
         <v>156</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>156</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>154</v>
       </c>
       <c r="G14" s="7" t="n">
         <v>1.5</v>
@@ -4960,7 +5161,7 @@
         <v>1</v>
       </c>
       <c r="M14" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4980,7 +5181,7 @@
         <v>0</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="G15" s="7" t="n">
         <v>1.5</v>
@@ -5001,7 +5202,7 @@
         <v>1</v>
       </c>
       <c r="M15" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5009,19 +5210,19 @@
         <v>20</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C16" s="7" t="n">
         <v>-50</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="E16" s="7" t="n">
         <v>-50</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="G16" s="7" t="n">
         <v>1.5</v>
@@ -5042,7 +5243,7 @@
         <v>1</v>
       </c>
       <c r="M16" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5062,7 +5263,7 @@
         <v>-50</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="G17" s="7" t="n">
         <v>1.5</v>
@@ -5083,7 +5284,7 @@
         <v>1</v>
       </c>
       <c r="M17" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5103,7 +5304,7 @@
         <v>0</v>
       </c>
       <c r="F18" s="19" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="G18" s="19" t="n">
         <v>1.5</v>
@@ -5124,7 +5325,7 @@
         <v>1</v>
       </c>
       <c r="M18" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5132,16 +5333,16 @@
         <v>23</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="F19" s="7" t="n">
         <v>1</v>
@@ -5165,7 +5366,7 @@
         <v>1</v>
       </c>
       <c r="M19" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5211,13 +5412,13 @@
         <v>25</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>-50</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="E21" s="0" t="n">
         <v>-50</v>
@@ -5366,7 +5567,7 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="0" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -5391,7 +5592,7 @@
       <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7"/>
@@ -5400,13 +5601,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>112</v>
@@ -5415,21 +5616,21 @@
         <v>113</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>50</v>
@@ -5440,16 +5641,16 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>172</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>170</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>50</v>
@@ -5460,16 +5661,16 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>50</v>
@@ -5480,16 +5681,16 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>50</v>
@@ -5500,16 +5701,16 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>0</v>
@@ -5540,7 +5741,7 @@
       <selection pane="topLeft" activeCell="R22" activeCellId="0" sqref="R22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="9.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="5.43"/>
@@ -5560,7 +5761,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="7.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="11.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="2" width="6.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="19" style="2" width="7.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="19" style="2" width="7.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="11.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="2" width="6.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="23" style="2" width="9.14"/>
@@ -5568,7 +5769,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>2</v>
@@ -5696,16 +5897,16 @@
         <v>24</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="G2" s="2" t="n">
         <v>1</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>29</v>
@@ -5714,7 +5915,7 @@
         <v>29</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>34</v>
@@ -5744,7 +5945,7 @@
         <v>34</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="V2" s="2" t="s">
         <v>34</v>
@@ -5756,7 +5957,7 @@
         <v>1</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="Z2" s="0" t="n">
         <v>1</v>
@@ -5773,7 +5974,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>2</v>
@@ -5782,10 +5983,10 @@
         <v>8</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="G3" s="2" t="n">
         <v>2</v>
@@ -5832,10 +6033,10 @@
         <v>64</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>42</v>
@@ -5876,10 +6077,10 @@
         <v>4</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>95</v>
@@ -5911,10 +6112,10 @@
         <v>5</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>39</v>

</xml_diff>